<commit_message>
fixed bug with LAOs and add fattyalcohols section
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/LAOs/results/Capital and operating costs.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/LAOs/results/Capital and operating costs.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/733a0933307f0df0/Code/Bioindustrial-Park/BioSTEAM 2.x.x/biorefineries/LAOs/results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{FD0ED853-52F9-4327-8B77-5F6D1ACBBE5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capital and operating costs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -106,25 +112,25 @@
     <t>Total variable operating cost</t>
   </si>
   <si>
+    <t>Tridecane</t>
+  </si>
+  <si>
     <t>Process water</t>
   </si>
   <si>
-    <t>Tridecane</t>
+    <t>Wastewater</t>
+  </si>
+  <si>
+    <t>Glucose</t>
+  </si>
+  <si>
+    <t>CSL</t>
   </si>
   <si>
     <t>DAP</t>
   </si>
   <si>
-    <t>Glucose</t>
-  </si>
-  <si>
     <t>Salt</t>
-  </si>
-  <si>
-    <t>CSL</t>
-  </si>
-  <si>
-    <t>Wastewater</t>
   </si>
   <si>
     <t>Natural gas</t>
@@ -154,8 +160,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,8 +213,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -218,6 +227,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -264,7 +281,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -296,9 +313,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -330,6 +365,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -505,14 +558,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -528,10 +581,10 @@
         <v>17</v>
       </c>
       <c r="C3">
-        <v>44.37578379219946</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>44.371165973952337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -539,10 +592,10 @@
         <v>17</v>
       </c>
       <c r="C4">
-        <v>26.51764973912804</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>26.53598744217307</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -550,10 +603,10 @@
         <v>18</v>
       </c>
       <c r="C5">
-        <v>1.775031351687978</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>1.774846638958093</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -561,10 +614,10 @@
         <v>19</v>
       </c>
       <c r="C6">
-        <v>3.993820541297951</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>3.9934049376557099</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -572,10 +625,10 @@
         <v>20</v>
       </c>
       <c r="C7">
-        <v>1.996910270648975</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>1.996702468827855</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -583,10 +636,10 @@
         <v>17</v>
       </c>
       <c r="C8">
-        <v>78.65919569496241</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>78.672107461567066</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -594,10 +647,10 @@
         <v>21</v>
       </c>
       <c r="C9">
-        <v>7.865919569496241</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>7.8672107461567071</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -605,10 +658,10 @@
         <v>21</v>
       </c>
       <c r="C10">
-        <v>7.865919569496241</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>7.8672107461567071</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -616,10 +669,10 @@
         <v>22</v>
       </c>
       <c r="C11">
-        <v>15.73183913899248</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>15.734421492313411</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -627,10 +680,10 @@
         <v>23</v>
       </c>
       <c r="C12">
-        <v>23.59775870848872</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>23.60163223847012</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -638,10 +691,10 @@
         <v>21</v>
       </c>
       <c r="C13">
-        <v>7.865919569496241</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>7.8672107461567071</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -649,10 +702,10 @@
         <v>17</v>
       </c>
       <c r="C14">
-        <v>62.92735655596994</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>62.937685969253643</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -660,10 +713,10 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>141.5865522509324</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>141.6097934308207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -671,10 +724,10 @@
         <v>24</v>
       </c>
       <c r="C16">
-        <v>7.079327612546618</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>7.0804896715410353</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -682,10 +735,10 @@
         <v>17</v>
       </c>
       <c r="C17">
-        <v>148.665879863479</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>148.69028310236169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
         <v>25</v>
       </c>
@@ -693,118 +746,118 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C21">
-        <v>0.320236305</v>
+        <v>775.64317499999993</v>
       </c>
       <c r="D21">
-        <v>0.3547184466667174</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1"/>
+        <v>-3.7139309833833033E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
       <c r="B22" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C22">
-        <v>775.6431749999999</v>
+        <v>0.320236305</v>
       </c>
       <c r="D22">
-        <v>-0.03714417253436945</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1"/>
+        <v>0.3544937424716692</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B23" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C23">
-        <v>895.3915949999999</v>
+        <v>-3.4222048137973369</v>
       </c>
       <c r="D23">
-        <v>0.4224116593363265</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1"/>
+        <v>-4.1054461435065672</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="B24" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C24">
-        <v>299.9970076499999</v>
+        <v>299.99700764999989</v>
       </c>
       <c r="D24">
         <v>160.5470037981996</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
       <c r="B25" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C25">
-        <v>136.07775</v>
+        <v>51.528108000000003</v>
       </c>
       <c r="D25">
-        <v>1.507665467094367</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1"/>
+        <v>0.2436875313576996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C26">
-        <v>51.528108</v>
+        <v>895.39159499999994</v>
       </c>
       <c r="D26">
-        <v>0.1949407114561928</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>0.42241247900968393</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C27">
-        <v>-3.186996033033347</v>
+        <v>136.07775000000001</v>
       </c>
       <c r="D27">
-        <v>-3.822518016581998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>1.5067104172463091</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C28">
-        <v>197.76633</v>
+        <v>197.76633000000001</v>
       </c>
       <c r="D28">
-        <v>3.02240149448353</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>3.0227578626756069</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="1"/>
       <c r="D29">
-        <v>169.8345154212844</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>170.16537266463331</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>0</v>
       </c>
@@ -815,7 +868,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -829,7 +882,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -843,7 +896,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -851,13 +904,13 @@
         <v>44</v>
       </c>
       <c r="C35">
-        <v>1.331273513765984</v>
+        <v>1.33113497921857</v>
       </c>
       <c r="D35">
-        <v>1.278022573215344</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>1.2778895800498269</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -865,15 +918,16 @@
         <v>44</v>
       </c>
       <c r="C36">
-        <v>0.3106304865453962</v>
+        <v>0.31059816181766642</v>
       </c>
       <c r="D36">
-        <v>0.2982052670835804</v>
+        <v>0.29817423534495968</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A21:A26"/>
+  <mergeCells count="2">
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A24:A28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>